<commit_message>
Discontinuidad en P, Kron, YRM
* Se agrego la discontinuidad en Potencia
* Ybus de falla
* YRM  ??
* VRM ??
</commit_message>
<xml_diff>
--- a/BUSDATA.xlsx
+++ b/BUSDATA.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo\Google Drive\Conversión y Transporte de Energía\CT4211 - Potencia III\SepDic2017 - Prof. Bermudez\Programas\Estabilidad-Transitoria-PIII\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11610" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11610" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="NODOS" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,7 @@
     <sheet name="GENERADORES" sheetId="3" r:id="rId5"/>
     <sheet name="INTEGRACION" sheetId="9" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -142,7 +137,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000000"/>
   </numFmts>
@@ -350,7 +345,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -385,7 +380,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -562,7 +557,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1231,8 +1226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1531,8 +1526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="A1:B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Eficticia, Pmec, fix a RM
* Arreglado YRMIRM
* Se calcula Eficiticia y angulo delta
* Se calcula Pmecanica y electrica
</commit_message>
<xml_diff>
--- a/BUSDATA.xlsx
+++ b/BUSDATA.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo\Google Drive\Conversión y Transporte de Energía\CT4211 - Potencia III\SepDic2017 - Prof. Bermudez\Programas\Estabilidad-Transitoria-PIII\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11610" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11610"/>
   </bookViews>
   <sheets>
     <sheet name="NODOS" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
     <sheet name="GENERADORES" sheetId="3" r:id="rId5"/>
     <sheet name="INTEGRACION" sheetId="9" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="39">
   <si>
     <t>BARRA</t>
   </si>
@@ -132,12 +137,21 @@
   </si>
   <si>
     <t>SHUNT /2</t>
+  </si>
+  <si>
+    <t>RA</t>
+  </si>
+  <si>
+    <t>XD</t>
+  </si>
+  <si>
+    <t>XQ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000000"/>
   </numFmts>
@@ -247,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -273,9 +287,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -285,6 +296,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,7 +574,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -567,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,7 +656,7 @@
       <c r="J2" s="2">
         <v>0</v>
       </c>
-      <c r="K2" s="12">
+      <c r="K2" s="11">
         <v>0</v>
       </c>
     </row>
@@ -674,7 +691,7 @@
       <c r="J3" s="2">
         <v>0</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="11">
         <v>0</v>
       </c>
     </row>
@@ -707,9 +724,9 @@
         <v>0</v>
       </c>
       <c r="J4" s="2">
-        <v>0</v>
-      </c>
-      <c r="K4" s="12">
+        <v>1</v>
+      </c>
+      <c r="K4" s="11">
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
@@ -724,7 +741,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="12"/>
+      <c r="K5" s="11"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -737,7 +754,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="12"/>
+      <c r="K6" s="11"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
@@ -750,7 +767,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="12"/>
+      <c r="K7" s="11"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
@@ -763,7 +780,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="12"/>
+      <c r="K8" s="11"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
@@ -776,7 +793,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="12"/>
+      <c r="K9" s="11"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
@@ -789,7 +806,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="12"/>
+      <c r="K10" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -801,7 +818,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="A1:H10"/>
+      <selection activeCell="B2" sqref="B2:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,7 +867,8 @@
         <v>0.1</v>
       </c>
       <c r="G2" s="2">
-        <v>0</v>
+        <f>F2/2</f>
+        <v>0.05</v>
       </c>
       <c r="H2" s="2">
         <v>1</v>
@@ -876,7 +894,8 @@
         <v>0.2</v>
       </c>
       <c r="G3" s="2">
-        <v>8.7999999999999995E-2</v>
+        <f t="shared" ref="G3:G5" si="0">F3/2</f>
+        <v>0.1</v>
       </c>
       <c r="H3" s="2">
         <v>1</v>
@@ -901,8 +920,9 @@
       <c r="F4" s="2">
         <v>0.3</v>
       </c>
-      <c r="G4" s="7">
-        <v>7.9000000000000001E-2</v>
+      <c r="G4" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
       </c>
       <c r="H4" s="7">
         <v>1</v>
@@ -928,7 +948,8 @@
         <v>0</v>
       </c>
       <c r="G5" s="2">
-        <v>0.153</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="H5" s="2">
         <v>1</v>
@@ -943,9 +964,7 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="2">
-        <v>0.17899999999999999</v>
-      </c>
+      <c r="G6" s="15"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -957,9 +976,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="2">
-        <v>7.4499999999999997E-2</v>
-      </c>
+      <c r="G7" s="15"/>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -971,9 +988,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="2">
-        <v>0.1045</v>
-      </c>
+      <c r="G8" s="15"/>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -985,9 +1000,7 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="2">
-        <v>0</v>
-      </c>
+      <c r="G9" s="15"/>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -999,13 +1012,12 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2">
-        <v>0</v>
-      </c>
+      <c r="G10" s="15"/>
       <c r="H10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1014,7 +1026,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H10"/>
+      <selection activeCell="B2" sqref="B2:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,7 +1075,8 @@
         <v>0.1</v>
       </c>
       <c r="G2" s="2">
-        <v>0</v>
+        <f>F2/2</f>
+        <v>0.05</v>
       </c>
       <c r="H2" s="2">
         <v>1</v>
@@ -1089,7 +1102,8 @@
         <v>0.2</v>
       </c>
       <c r="G3" s="2">
-        <v>8.7999999999999995E-2</v>
+        <f t="shared" ref="G3:G5" si="0">F3/2</f>
+        <v>0.1</v>
       </c>
       <c r="H3" s="2">
         <v>1</v>
@@ -1114,8 +1128,9 @@
       <c r="F4" s="2">
         <v>0.3</v>
       </c>
-      <c r="G4" s="7">
-        <v>7.9000000000000001E-2</v>
+      <c r="G4" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
       </c>
       <c r="H4" s="7">
         <v>1</v>
@@ -1141,7 +1156,8 @@
         <v>0</v>
       </c>
       <c r="G5" s="2">
-        <v>0.153</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="H5" s="2">
         <v>1</v>
@@ -1156,9 +1172,7 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="2">
-        <v>0.17899999999999999</v>
-      </c>
+      <c r="G6" s="15"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1170,9 +1184,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="2">
-        <v>7.4499999999999997E-2</v>
-      </c>
+      <c r="G7" s="15"/>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1184,9 +1196,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="2">
-        <v>0.1045</v>
-      </c>
+      <c r="G8" s="15"/>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1198,9 +1208,7 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="2">
-        <v>0</v>
-      </c>
+      <c r="G9" s="15"/>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1212,9 +1220,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2">
-        <v>0</v>
-      </c>
+      <c r="G10" s="15"/>
       <c r="H10" s="2"/>
     </row>
   </sheetData>
@@ -1227,7 +1233,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="B2" sqref="B2:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1276,7 +1282,8 @@
         <v>0.1</v>
       </c>
       <c r="G2" s="2">
-        <v>0</v>
+        <f>F2/2</f>
+        <v>0.05</v>
       </c>
       <c r="H2" s="2">
         <v>1</v>
@@ -1302,7 +1309,8 @@
         <v>0.2</v>
       </c>
       <c r="G3" s="2">
-        <v>8.7999999999999995E-2</v>
+        <f t="shared" ref="G3:G5" si="0">F3/2</f>
+        <v>0.1</v>
       </c>
       <c r="H3" s="2">
         <v>1</v>
@@ -1327,8 +1335,9 @@
       <c r="F4" s="2">
         <v>0.3</v>
       </c>
-      <c r="G4" s="7">
-        <v>7.9000000000000001E-2</v>
+      <c r="G4" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
       </c>
       <c r="H4" s="7">
         <v>1</v>
@@ -1354,7 +1363,8 @@
         <v>0</v>
       </c>
       <c r="G5" s="2">
-        <v>0.153</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="H5" s="2">
         <v>1</v>
@@ -1369,9 +1379,7 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="2">
-        <v>0.17899999999999999</v>
-      </c>
+      <c r="G6" s="15"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1383,9 +1391,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="2">
-        <v>7.4499999999999997E-2</v>
-      </c>
+      <c r="G7" s="15"/>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1397,9 +1403,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="2">
-        <v>0.1045</v>
-      </c>
+      <c r="G8" s="15"/>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1411,9 +1415,7 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="2">
-        <v>0</v>
-      </c>
+      <c r="G9" s="15"/>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1425,9 +1427,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2">
-        <v>0</v>
-      </c>
+      <c r="G10" s="15"/>
       <c r="H10" s="2"/>
     </row>
   </sheetData>
@@ -1440,81 +1440,108 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
+      <c r="G1" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
-        <v>1</v>
-      </c>
-      <c r="B2" s="11">
-        <v>0</v>
-      </c>
-      <c r="C2" s="11">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10">
+        <v>0</v>
+      </c>
+      <c r="C2" s="10">
         <v>0.1</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="10">
         <v>-1</v>
       </c>
-      <c r="E2" s="11">
-        <v>0</v>
-      </c>
-      <c r="F2" s="11">
+      <c r="E2" s="10">
+        <v>0</v>
+      </c>
+      <c r="F2" s="10">
         <v>4</v>
       </c>
+      <c r="G2" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="H2" s="10">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I2" s="10">
+        <v>2.2000000000000002</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
+      <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3" s="11">
-        <v>0</v>
-      </c>
-      <c r="C3" s="11">
+      <c r="B3" s="10">
+        <v>0</v>
+      </c>
+      <c r="C3" s="10">
         <v>0.12</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="10">
         <v>-1</v>
       </c>
-      <c r="E3" s="11">
-        <v>0</v>
-      </c>
-      <c r="F3" s="11">
+      <c r="E3" s="10">
+        <v>0</v>
+      </c>
+      <c r="F3" s="10">
         <v>5</v>
       </c>
+      <c r="G3" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H3" s="10">
+        <v>2.15</v>
+      </c>
+      <c r="I3" s="10">
+        <v>2.23</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1526,7 +1553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1536,48 +1563,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="14">
+      <c r="B1" s="13">
         <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="13">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="13">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="13">
         <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="13">
         <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="14"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>